<commit_message>
count2:adding CD4 count result in lab test
</commit_message>
<xml_diff>
--- a/config/forms/app/lab.xlsx
+++ b/config/forms/app/lab.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="94">
   <si>
     <t>type</t>
   </si>
@@ -154,6 +154,18 @@
     <t>${result} = 'yes'</t>
   </si>
   <si>
+    <t>select_one snooze</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This patient should be scheduled for a CD4 Lab count based on their result and date of last lab appointment. </t>
+  </si>
+  <si>
+    <t>${count} = 'unstable' or ${count} = 'stable' or ${count} = 'inconclusive' or ${count} = 'unknown'</t>
+  </si>
+  <si>
     <t>select_one load</t>
   </si>
   <si>
@@ -161,6 +173,9 @@
   </si>
   <si>
     <t>Viral Load:</t>
+  </si>
+  <si>
+    <t>${result} = 'yes' and ${test} = 'viral'</t>
   </si>
   <si>
     <t>list_name</t>
@@ -197,17 +212,30 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>unsuppressed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unsuppressed (CD4 count is below 350 cells/mm3)
+    <t>stable</t>
+  </si>
+  <si>
+    <t>Stable or Suppressed (CD4 count is 350 or above 350 cells/mm3)</t>
+  </si>
+  <si>
+    <t>unstable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unstable or Unsuppressed 
+(CD4 count is below 350 cells/mm3)
 </t>
   </si>
   <si>
-    <t>suppressed</t>
-  </si>
-  <si>
-    <t>Suppressed (CD4 count is 350 or above 350 cells/mm3)</t>
+    <t>inconclusive</t>
+  </si>
+  <si>
+    <t>Inconclusive (Lab test did not work, so patient will need to have a new lab test appointment)</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Unknown / no result (Lab test did not give a result. Close this Task and set up new lab test appointment for patient)</t>
   </si>
   <si>
     <t>unsuppressed1</t>
@@ -222,6 +250,21 @@
   <si>
     <t xml:space="preserve">Suppressed Viral Load      (viral load is below 1,000 copies/ml)
 </t>
+  </si>
+  <si>
+    <t>snooze</t>
+  </si>
+  <si>
+    <t>snooze1</t>
+  </si>
+  <si>
+    <t>Okay,I will schedule an appointment for a lab visit</t>
+  </si>
+  <si>
+    <t>snooze2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remind me to schedule an appointment in 2 days </t>
   </si>
   <si>
     <t>form_title</t>
@@ -608,8 +651,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="29.63"/>
-    <col customWidth="1" min="3" max="3" width="29.25"/>
-    <col customWidth="1" min="4" max="4" width="25.5"/>
+    <col customWidth="1" min="3" max="3" width="81.5"/>
+    <col customWidth="1" min="4" max="4" width="72.5"/>
     <col customWidth="1" min="6" max="6" width="21.0"/>
   </cols>
   <sheetData>
@@ -1003,11 +1046,25 @@
         <v>48</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1026,12 +1083,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="50.25"/>
+    <col customWidth="1" min="3" max="3" width="84.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1068,10 +1125,10 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
@@ -1079,10 +1136,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
@@ -1090,10 +1147,10 @@
         <v>40</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1101,10 +1158,10 @@
         <v>40</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
@@ -1112,10 +1169,10 @@
         <v>40</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -1123,10 +1180,10 @@
         <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8">
@@ -1134,32 +1191,76 @@
         <v>43</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>67</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1179,47 +1280,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C2" s="11" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-06-29_22-36</v>
+        <v>2022-07-11_09-27</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
referral:changing the lat test result to CD4 lab test result
</commit_message>
<xml_diff>
--- a/config/forms/app/lab.xlsx
+++ b/config/forms/app/lab.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
   <si>
     <t>type</t>
   </si>
@@ -117,7 +117,7 @@
     <t>appoint</t>
   </si>
   <si>
-    <t>select_one test or_other</t>
+    <t xml:space="preserve">select_one test </t>
   </si>
   <si>
     <t>test</t>
@@ -188,12 +188,6 @@
 </t>
   </si>
   <si>
-    <t>viral</t>
-  </si>
-  <si>
-    <t>Viral Load</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -209,7 +203,7 @@
     <t>un</t>
   </si>
   <si>
-    <t>Unknown</t>
+    <t>Unknown (Lab test did not give a result after 14 days. Close this Task and set up new lab test appointment for patient to get a new lab draw)</t>
   </si>
   <si>
     <t>stable</t>
@@ -229,13 +223,7 @@
     <t>inconclusive</t>
   </si>
   <si>
-    <t>Inconclusive (Lab test did not work, so patient will need to have a new lab test appointment)</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>Unknown / no result (Lab test did not give a result. Close this Task and set up new lab test appointment for patient)</t>
+    <t xml:space="preserve">Inconclusive </t>
   </si>
   <si>
     <t>unsuppressed1</t>
@@ -258,13 +246,14 @@
     <t>snooze1</t>
   </si>
   <si>
-    <t>Okay,I will schedule an appointment for a lab visit</t>
+    <t xml:space="preserve">Okay, I will schedule a CD4 Lab Appointment
+</t>
   </si>
   <si>
     <t>snooze2</t>
   </si>
   <si>
-    <t xml:space="preserve">Remind me to schedule an appointment in 2 days </t>
+    <t xml:space="preserve">Keep this reminder in my Task List </t>
   </si>
   <si>
     <t>form_title</t>
@@ -288,7 +277,7 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>Lab Test Result</t>
+    <t>CD4 Lab Test Result</t>
   </si>
   <si>
     <t>lab</t>
@@ -1083,7 +1072,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="84.63"/>
+    <col customWidth="1" min="3" max="3" width="103.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1133,7 +1122,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>57</v>
@@ -1166,7 +1155,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>63</v>
@@ -1199,7 +1188,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>69</v>
@@ -1210,7 +1199,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>71</v>
@@ -1221,46 +1210,24 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1277,50 +1244,53 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.88"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" s="11" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-11_09-27</v>
+        <v>2022-07-13_10-47</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
viral-task:configuring when a new appointment task should re-appear in CD4 Lab Test Result and Viral Load Lab Test Result
</commit_message>
<xml_diff>
--- a/config/forms/app/lab.xlsx
+++ b/config/forms/app/lab.xlsx
@@ -39,7 +39,7 @@
     <t>inputs</t>
   </si>
   <si>
-    <t xml:space="preserve"> New Task Form</t>
+    <t>CD4 Lab Test Result</t>
   </si>
   <si>
     <t>./source = 'user'</t>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>appoint1</t>
   </si>
   <si>
     <t>Date of Appointment</t>
@@ -275,9 +278,6 @@
   </si>
   <si>
     <t>default_language</t>
-  </si>
-  <si>
-    <t>CD4 Lab Test Result</t>
   </si>
   <si>
     <t>lab</t>
@@ -375,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -384,6 +384,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -672,7 +675,7 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -684,13 +687,13 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="2"/>
@@ -700,13 +703,13 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2"/>
@@ -716,13 +719,13 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2"/>
@@ -730,13 +733,13 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2"/>
@@ -746,13 +749,13 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2"/>
@@ -762,13 +765,13 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2"/>
@@ -778,13 +781,13 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2"/>
@@ -794,13 +797,13 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2"/>
@@ -810,13 +813,13 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2"/>
@@ -824,13 +827,13 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2"/>
@@ -838,13 +841,13 @@
       <c r="F12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2"/>
@@ -854,13 +857,13 @@
       <c r="F13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2"/>
@@ -870,82 +873,82 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -978,82 +981,82 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="C23" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="C24" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="8" t="s">
         <v>45</v>
       </c>
+      <c r="D25" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>49</v>
       </c>
+      <c r="D26" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="C27" s="8" t="s">
         <v>53</v>
       </c>
+      <c r="D27" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1077,7 +1080,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1110,124 +1113,124 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>56</v>
       </c>
+      <c r="C2" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>58</v>
       </c>
+      <c r="C3" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="A4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>60</v>
       </c>
+      <c r="C4" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="A5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>62</v>
       </c>
+      <c r="C5" s="8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="A6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>64</v>
       </c>
+      <c r="C6" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="A7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>66</v>
       </c>
+      <c r="C7" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>68</v>
       </c>
+      <c r="C8" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>70</v>
       </c>
+      <c r="C9" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>72</v>
       </c>
+      <c r="C10" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>75</v>
       </c>
+      <c r="C11" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="A12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>77</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1250,46 +1253,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>84</v>
       </c>
+      <c r="G1" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="11" t="str">
+      <c r="C2" s="12" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-13_10-47</v>
-      </c>
-      <c r="D2" s="12" t="s">
+        <v>2022-07-18_11-47</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
auto:change to data dashboard and setting a task reminder
</commit_message>
<xml_diff>
--- a/config/forms/app/lab.xlsx
+++ b/config/forms/app/lab.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
   <si>
     <t>type</t>
   </si>
@@ -60,6 +60,15 @@
     <t>source_id</t>
   </si>
   <si>
+    <t xml:space="preserve">hidden </t>
+  </si>
+  <si>
+    <t>my_field_lab</t>
+  </si>
+  <si>
+    <t>lab_field_date</t>
+  </si>
+  <si>
     <t>contact</t>
   </si>
   <si>
@@ -117,22 +126,19 @@
     <t>appoint</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one test </t>
+    <t>note</t>
   </si>
   <si>
     <t>test</t>
   </si>
   <si>
-    <t>Lab test:</t>
-  </si>
-  <si>
-    <t>date</t>
+    <t>Lab test: ${my_field_lab}</t>
   </si>
   <si>
     <t>appoint1</t>
   </si>
   <si>
-    <t>Date of Appointment</t>
+    <t>Date of Appointment: ${lab_field_date}</t>
   </si>
   <si>
     <t>select_one result</t>
@@ -182,13 +188,6 @@
   </si>
   <si>
     <t>list_name</t>
-  </si>
-  <si>
-    <t>cd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4 count
-</t>
   </si>
   <si>
     <t>yes</t>
@@ -375,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -393,6 +392,12 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -720,12 +725,12 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2"/>
@@ -733,59 +738,55 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>13</v>
@@ -798,10 +799,10 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
@@ -813,88 +814,100 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>24</v>
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>15</v>
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
+      <c r="A13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>1</v>
+      <c r="A14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>26</v>
+      <c r="A17" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -903,8 +916,8 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>26</v>
+      <c r="A18" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -913,151 +926,171 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="A19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="8" t="s">
+    </row>
+    <row r="23">
+      <c r="A23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="8" t="s">
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B24" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C24" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="8" t="s">
+    <row r="25">
+      <c r="A25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="8" t="s">
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="8" t="s">
+      <c r="B26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="8" t="s">
+    </row>
+    <row r="27">
+      <c r="A27" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="B27" s="10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="8" t="s">
+      <c r="C27" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="D27" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="8" t="s">
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="B28" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="8" t="s">
+      <c r="C28" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="D28" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="8" t="s">
+    </row>
+    <row r="29">
+      <c r="A29" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="B29" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="8" t="s">
-        <v>26</v>
+      <c r="C29" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1113,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1113,123 +1146,112 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>57</v>
+      <c r="A2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>59</v>
+      <c r="A3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>61</v>
+      <c r="A4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>63</v>
+      <c r="A5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>65</v>
+      <c r="A6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>67</v>
+      <c r="A7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>69</v>
+      <c r="A8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>71</v>
+      <c r="A9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>73</v>
+      <c r="A10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C11" s="10" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1261,38 +1283,38 @@
       <c r="C1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="12" t="str">
+      <c r="C2" s="14" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-18_11-47</v>
-      </c>
-      <c r="D2" s="13" t="s">
+        <v>2022-07-25_15-59</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>